<commit_message>
correção no prazo de arquivo
</commit_message>
<xml_diff>
--- a/Guidelines/guidelines_SCAP_fornecedoresAtributos.xlsx
+++ b/Guidelines/guidelines_SCAP_fornecedoresAtributos.xlsx
@@ -1131,7 +1131,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> garantir que o FA arquiva a informação necessária que permite reconstruir a autorização para adição e remoção do atributo da base de dados de atributos, durante um período de 17 anos.
+      <t xml:space="preserve"> garantir que o FA arquiva a informação necessária que permite reconstruir a autorização para adição e remoção do atributo da base de dados de atributos, durante um período de 10 anos.
 </t>
     </r>
     <r>
@@ -1151,7 +1151,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> indicar o processo/procedimento utilizado pelo FA para arquivar a informação necessária que permite reconstruir a autorização para adição e remoção do atributo da base de dados de atributos, durante um período de 17 anos.</t>
+      <t xml:space="preserve"> indicar o processo/procedimento utilizado pelo FA para arquivar a informação necessária que permite reconstruir a autorização para adição e remoção do atributo da base de dados de atributos, durante um período de 10 anos.</t>
     </r>
   </si>
   <si>
@@ -1178,7 +1178,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> garantir que pedidos de assinatura de atributo e respetiva resposta, são arquivados durante um período de 17 anos.
+      <t xml:space="preserve"> garantir que pedidos de assinatura de atributo e respetiva resposta, são arquivados durante um período de 10 anos.
 </t>
     </r>
     <r>
@@ -1198,7 +1198,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> indicar que autoriza a AMA a arquivar o pedido de atributo e respetiva resposta, durante um período de 17 anos.</t>
+      <t xml:space="preserve"> indicar que autoriza a AMA a arquivar o pedido de atributo e respetiva resposta, durante um período de 10 anos.</t>
     </r>
   </si>
   <si>
@@ -1564,7 +1564,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1611,10 +1611,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1725,19 +1721,17 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="F2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="F19" activeCellId="0" sqref="F19"/>
+      <selection pane="bottomLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="33.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="79.43"/>
   </cols>
@@ -2118,7 +2112,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" s="12" customFormat="true" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="n">
         <f aca="false">A18+1</f>
         <v>18</v>
@@ -2139,7 +2133,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" s="12" customFormat="true" ht="105.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="105.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="n">
         <f aca="false">A19+1</f>
         <v>19</v>
@@ -2159,9 +2153,9 @@
       <c r="F20" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="G20" s="13"/>
-    </row>
-    <row r="21" s="12" customFormat="true" ht="120.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G20" s="12"/>
+    </row>
+    <row r="21" customFormat="false" ht="120.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="n">
         <f aca="false">A20+1</f>
         <v>20</v>
@@ -2181,9 +2175,9 @@
       <c r="F21" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="G21" s="13"/>
-    </row>
-    <row r="22" s="12" customFormat="true" ht="90.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G21" s="12"/>
+    </row>
+    <row r="22" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="n">
         <f aca="false">A21+1</f>
         <v>21</v>
@@ -2203,9 +2197,9 @@
       <c r="F22" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="G22" s="13"/>
-    </row>
-    <row r="23" s="12" customFormat="true" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G22" s="12"/>
+    </row>
+    <row r="23" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="n">
         <f aca="false">A22+1</f>
         <v>22</v>
@@ -2225,9 +2219,9 @@
       <c r="F23" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="G23" s="14"/>
-    </row>
-    <row r="24" s="12" customFormat="true" ht="60.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G23" s="13"/>
+    </row>
+    <row r="24" customFormat="false" ht="60.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="n">
         <f aca="false">A23+1</f>
         <v>23</v>
@@ -2247,9 +2241,9 @@
       <c r="F24" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="G24" s="13"/>
-    </row>
-    <row r="25" s="12" customFormat="true" ht="60.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G24" s="12"/>
+    </row>
+    <row r="25" customFormat="false" ht="60.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="n">
         <f aca="false">A24+1</f>
         <v>24</v>
@@ -2269,9 +2263,9 @@
       <c r="F25" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="G25" s="13"/>
-    </row>
-    <row r="26" s="12" customFormat="true" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G25" s="12"/>
+    </row>
+    <row r="26" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="10" t="n">
         <f aca="false">A25+1</f>
         <v>25</v>
@@ -2306,39 +2300,38 @@
       <c r="D27" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="E27" s="14" t="s">
         <v>90</v>
       </c>
       <c r="F27" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="G27" s="12"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="16"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="18"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="17"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="18"/>
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="17"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="16"/>
-      <c r="B30" s="19" t="s">
+      <c r="A30" s="15"/>
+      <c r="B30" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="18"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="17"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>